<commit_message>
added gitignore and modified runtime file
</commit_message>
<xml_diff>
--- a/runtime.xlsx
+++ b/runtime.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\path-puzzles-sat-solver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B666AF-04B8-4EE3-8540-1A7823D899F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBD240A-5479-4B1E-990B-9237EDFAF62D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10155" yWindow="2580" windowWidth="18645" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="1425" windowWidth="18645" windowHeight="12225" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="backtracking" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="39">
   <si>
     <t>A</t>
   </si>
@@ -138,9 +138,6 @@
     <t>ADDITIONAL CASES</t>
   </si>
   <si>
-    <t>6x6</t>
-  </si>
-  <si>
     <t>7x7</t>
   </si>
   <si>
@@ -154,9 +151,6 @@
   </si>
   <si>
     <t>11x11</t>
-  </si>
-  <si>
-    <t>12x12</t>
   </si>
   <si>
     <t>timeout</t>
@@ -514,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1057,35 +1051,35 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>415.65699999999998</v>
+        <v>35668.699999999997</v>
       </c>
       <c r="C34">
-        <v>493.81299999999999</v>
+        <v>35468.300000000003</v>
       </c>
       <c r="D34">
-        <v>512.58900000000006</v>
+        <v>36261.300000000003</v>
       </c>
       <c r="E34">
-        <f>AVERAGE(B34:D34)</f>
-        <v>474.01966666666675</v>
+        <f t="shared" ref="E34:E38" si="1">AVERAGE(B34:D34)</f>
+        <v>35799.433333333334</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B35">
-        <v>35668.699999999997</v>
-      </c>
-      <c r="C35">
-        <v>35468.300000000003</v>
-      </c>
-      <c r="D35">
-        <v>36261.300000000003</v>
-      </c>
-      <c r="E35">
-        <f t="shared" ref="E35:E39" si="1">AVERAGE(B35:D35)</f>
-        <v>35799.433333333334</v>
+      <c r="B35" t="s">
+        <v>38</v>
+      </c>
+      <c r="C35" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1093,13 +1087,13 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D36" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E36" t="e">
         <f t="shared" si="1"/>
@@ -1111,13 +1105,13 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D37" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E37" t="e">
         <f t="shared" si="1"/>
@@ -1129,52 +1123,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D38" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E38" t="e">
         <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>40</v>
-      </c>
-      <c r="C39" t="s">
-        <v>40</v>
-      </c>
-      <c r="D39" t="s">
-        <v>40</v>
-      </c>
-      <c r="E39" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" t="s">
-        <v>40</v>
-      </c>
-      <c r="E40" t="e">
-        <f t="shared" ref="E40" si="2">AVERAGE(B40:D40)</f>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -1192,10 +1150,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AEA177E-4420-44BB-938C-61B02795712B}">
-  <dimension ref="A1:E40"/>
+  <dimension ref="A1:E38"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,17 +1693,17 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>60.091000000000001</v>
+        <v>153.94399999999999</v>
       </c>
       <c r="C34">
-        <v>62.110999999999997</v>
+        <v>142.36199999999999</v>
       </c>
       <c r="D34">
-        <v>61.103999999999999</v>
+        <v>148.874</v>
       </c>
       <c r="E34">
-        <f>AVERAGE(B34:D34)</f>
-        <v>61.101999999999997</v>
+        <f t="shared" ref="E34:E38" si="1">AVERAGE(B34:D34)</f>
+        <v>148.39333333333332</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1753,17 +1711,17 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>153.94399999999999</v>
+        <v>315.70499999999998</v>
       </c>
       <c r="C35">
-        <v>142.36199999999999</v>
+        <v>311.471</v>
       </c>
       <c r="D35">
-        <v>148.874</v>
+        <v>316.34399999999999</v>
       </c>
       <c r="E35">
-        <f t="shared" ref="E35:E40" si="1">AVERAGE(B35:D35)</f>
-        <v>148.39333333333332</v>
+        <f t="shared" si="1"/>
+        <v>314.50666666666666</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1771,17 +1729,17 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>315.70499999999998</v>
+        <v>727.51300000000003</v>
       </c>
       <c r="C36">
-        <v>311.471</v>
+        <v>705.13499999999999</v>
       </c>
       <c r="D36">
-        <v>316.34399999999999</v>
+        <v>749.37400000000002</v>
       </c>
       <c r="E36">
         <f t="shared" si="1"/>
-        <v>314.50666666666666</v>
+        <v>727.34066666666661</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1789,17 +1747,17 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>727.51300000000003</v>
+        <v>1968.6780000000001</v>
       </c>
       <c r="C37">
-        <v>705.13499999999999</v>
+        <v>1735.9849999999999</v>
       </c>
       <c r="D37">
-        <v>749.37400000000002</v>
+        <v>1725.9469999999999</v>
       </c>
       <c r="E37">
         <f t="shared" si="1"/>
-        <v>727.34066666666661</v>
+        <v>1810.2033333333331</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,53 +1765,17 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>1968.6780000000001</v>
+        <v>3666.7020000000002</v>
       </c>
       <c r="C38">
-        <v>1735.9849999999999</v>
+        <v>3861.6770000000001</v>
       </c>
       <c r="D38">
-        <v>1725.9469999999999</v>
+        <v>3415.5219999999999</v>
       </c>
       <c r="E38">
         <f t="shared" si="1"/>
-        <v>1810.2033333333331</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39">
-        <v>3666.7020000000002</v>
-      </c>
-      <c r="C39">
-        <v>3861.6770000000001</v>
-      </c>
-      <c r="D39">
-        <v>3415.5219999999999</v>
-      </c>
-      <c r="E39">
-        <f t="shared" si="1"/>
         <v>3647.9670000000006</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40">
-        <v>14395.874</v>
-      </c>
-      <c r="C40">
-        <v>15678.287</v>
-      </c>
-      <c r="D40">
-        <v>16060.957</v>
-      </c>
-      <c r="E40">
-        <f t="shared" si="1"/>
-        <v>15378.372666666668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>